<commit_message>
Final Completed Version of Expense Tracker v0.1
</commit_message>
<xml_diff>
--- a/server/ExpenseData.xlsx
+++ b/server/ExpenseData.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,18 +416,29 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Food</v>
+        <v>Groceries</v>
       </c>
       <c r="B2">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
-        <v>45959.21608796297</v>
+        <v>45965.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Spotify Subscription</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45965.22928240741</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>